<commit_message>
Se actualiza diagrama de Gantt y se agrega el Usuario de prueba de Paypal
</commit_message>
<xml_diff>
--- a/Diagrama Gantt Tecnoventas.xlsx
+++ b/Diagrama Gantt Tecnoventas.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Tecnoventas-document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FAA22B-F8D0-4285-A1E7-C1D4E2FCB17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41EA3DB-5960-400F-BC40-84D2343552E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>Santiago</t>
   </si>
@@ -181,9 +170,6 @@
   </si>
   <si>
     <t>Generar PDF Del Pedido</t>
-  </si>
-  <si>
-    <t>Actualizar Cantidad Del Producto En El Carrito</t>
   </si>
 </sst>
 </file>
@@ -194,7 +180,7 @@
     <numFmt numFmtId="164" formatCode="dd"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -269,6 +255,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,6 +495,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2290,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D32" s="43">
         <v>45345</v>
@@ -2299,22 +2297,12 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D33" s="43">
-        <v>45345</v>
-      </c>
-      <c r="E33" s="43">
-        <v>45352</v>
-      </c>
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2352,11 +2340,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:AH28">
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(G$5&gt;=$D7,G$5&lt;=$E7)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C30">
     <cfRule type="dataBar" priority="1">
       <dataBar>
@@ -2381,6 +2364,11 @@
           <x14:id>{BDCCE43A-A470-44BD-B4ED-0A702F534F89}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:AH28">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>AND(G$5&gt;=$D7,G$5&lt;=$E7)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>